<commit_message>
Ping monitor stabil hale getirildi
</commit_message>
<xml_diff>
--- a/devices.xlsx
+++ b/devices.xlsx
@@ -1,102 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aysenurdemirci/PingMonitor/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2132C09-969B-A74F-88A1-523E55ADE3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16560" xr2:uid="{FE95DC6A-B72F-6148-BF51-216A04C45117}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16560" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sayfa1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>ip</t>
-  </si>
-  <si>
-    <t>a_1</t>
-  </si>
-  <si>
-    <t>8.8.8.8</t>
-  </si>
-  <si>
-    <t>b_2</t>
-  </si>
-  <si>
-    <t>2.2.2.2</t>
-  </si>
-  <si>
-    <t>c_2</t>
-  </si>
-  <si>
-    <t>3.3.3.3</t>
-  </si>
-  <si>
-    <t>d_1</t>
-  </si>
-  <si>
-    <t>149.140.146.212</t>
-  </si>
-  <si>
-    <t>208.67.222.222</t>
-  </si>
-  <si>
-    <t>e_1</t>
-  </si>
-  <si>
-    <t>9.9.9.9</t>
-  </si>
-  <si>
-    <t>f_1</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Aptos Narrow"/>
+      <charset val="162"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -115,22 +47,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -450,73 +441,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C417A9-E9D1-954D-AB02-E40E0ECC9698}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col width="14.6640625" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Device Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Device</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MAC</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Unit</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a_1</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>b_2</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>2.2.2.2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dfgfd</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ayse</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>qaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>c_2</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>3.3.3.3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dfgfd</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ayse1</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>fgv</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>cxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>d_1</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>149.140.146.212</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dfgfd</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>bv</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>e_1</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>208.67.222.222</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dfgfd</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>fdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>10.20.30.40</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fg</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>f_2</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>1.1.1.2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dfgfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>5.5.5.5</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>